<commit_message>
[Refactor] 변수명 통일 중 - name을 displayName/EnemyName으로 통일, player를 character로 통일
</commit_message>
<xml_diff>
--- a/characterCardLevelInfo_data.xlsx
+++ b/characterCardLevelInfo_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="11460"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="6780"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -43,6 +43,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <x:si>
+    <x:t>이동속도를 {0}만큼 증가시킵니다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공격속도를 {0}만큼 증가시킵니다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>공격력을 {0}만큼 증가시킵니다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>increase</x:t>
+  </x:si>
+  <x:si>
+    <x:t>description</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> ~ 스킬을 획득합니다.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>~ 스킬을 획득합니다.</x:t>
+  </x:si>
+  <x:si>
     <x:t>흔한4</x:t>
   </x:si>
   <x:si>
@@ -55,82 +76,61 @@
     <x:t>흔한9</x:t>
   </x:si>
   <x:si>
+    <x:t>주몽6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주몽4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주몽2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주몽3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주몽9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>흔한2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>흔한5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주몽5</x:t>
+  </x:si>
+  <x:si>
     <x:t>흔한8</x:t>
   </x:si>
   <x:si>
-    <x:t>흔한5</x:t>
-  </x:si>
-  <x:si>
     <x:t>흔한7</x:t>
   </x:si>
   <x:si>
-    <x:t>주몽2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주몽6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주몽5</x:t>
-  </x:si>
-  <x:si>
     <x:t>주몽8</x:t>
   </x:si>
   <x:si>
-    <x:t>주몽4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주몽9</x:t>
-  </x:si>
-  <x:si>
     <x:t>주몽7</x:t>
   </x:si>
   <x:si>
-    <x:t>주몽3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공격력을 {0}만큼 증가시킵니다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이동속도를 {0}만큼 증가시킵니다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>공격속도를 {0}만큼 증가시킵니다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>~ 스킬을 획득합니다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> ~ 스킬을 획득합니다.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>흔한2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>increase</x:t>
-  </x:si>
-  <x:si>
-    <x:t>description</x:t>
+    <x:t>display_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주몽10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>string</x:t>
+  </x:si>
+  <x:si>
+    <x:t>흔한11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>흔한10</x:t>
   </x:si>
   <x:si>
     <x:t>주몽11</x:t>
   </x:si>
   <x:si>
     <x:t>float</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주몽10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>string</x:t>
-  </x:si>
-  <x:si>
-    <x:t>흔한10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>흔한11</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -575,12 +575,12 @@
   <x:dimension ref="A1:C22"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="A1" activeCellId="0" sqref="A1:C22"/>
+      <x:selection activeCell="E4" activeCellId="0" sqref="E4:E4"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.39999999999999857891"/>
   <x:cols>
-    <x:col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="12.52734375" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="7.96875" bestFit="1" customWidth="1"/>
     <x:col min="3" max="3" width="33.41015625" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
@@ -590,35 +590,35 @@
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="A1" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3">
       <x:c r="A2" s="2" t="s">
-        <x:v>27</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>27</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
       <x:c r="A3" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B3" s="3">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C3" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
@@ -629,205 +629,205 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="C4" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B5" s="3">
         <x:v>0</x:v>
       </x:c>
       <x:c r="C5" s="3" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="3" t="s">
-        <x:v>9</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B6" s="3">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="3" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B7" s="3">
         <x:v>0</x:v>
       </x:c>
       <x:c r="C7" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="3" t="s">
-        <x:v>13</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B8" s="3">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C8" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="3" t="s">
-        <x:v>10</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B9" s="3">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C9" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B10" s="3">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C10" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="3" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B11" s="3">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C11" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="3" t="s">
-        <x:v>23</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B12" s="3">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C12" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B13" s="3">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C13" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="A14" s="3" t="s">
-        <x:v>2</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B14" s="3">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C14" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="A15" s="3" t="s">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B15" s="3">
         <x:v>0</x:v>
       </x:c>
       <x:c r="C15" s="3" t="s">
-        <x:v>18</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B16" s="3">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C16" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="3" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B17" s="3">
         <x:v>0</x:v>
       </x:c>
       <x:c r="C17" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="3" t="s">
-        <x:v>6</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B18" s="3">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C18" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="3" t="s">
-        <x:v>4</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B19" s="3">
         <x:v>5</x:v>
       </x:c>
       <x:c r="C19" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="3" t="s">
-        <x:v>3</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B20" s="3">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C20" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="3" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B21" s="3">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C21" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B22" s="3">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C22" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>